<commit_message>
opzetten van database + models3 + eerste functionaliteite homecontroller+view
</commit_message>
<xml_diff>
--- a/erp.xlsx
+++ b/erp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>wedstrijd deelnemer</t>
   </si>
@@ -75,14 +75,44 @@
   </si>
   <si>
     <t>gekwalificeerd</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>wedstrijd fk</t>
+  </si>
+  <si>
+    <t>wedstrijdeelnemer fk</t>
+  </si>
+  <si>
+    <t>wedstrijdverantwoordelijke fk</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
+  <si>
+    <t>wachtwoord</t>
+  </si>
+  <si>
+    <t>ww</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -219,6 +249,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -533,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:N22"/>
+  <dimension ref="D7:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,87 +656,125 @@
       <c r="L12" t="s">
         <v>3</v>
       </c>
+      <c r="N12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K16" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="13" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
-      <c r="K16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>15</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="N19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
       <c r="M20" s="3"/>
-      <c r="N20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
       <c r="K21" s="12" t="s">
         <v>6</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="5"/>
-      <c r="N21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K22" s="6"/>
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
-      <c r="N22" t="s">
+    </row>
+    <row r="24" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="L24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="L25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="L27" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>